<commit_message>
Update: test plan and test cases
</commit_message>
<xml_diff>
--- a/docs/test_plan.xlsx
+++ b/docs/test_plan.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F5F4E-973B-4BD5-9366-8323DD8B09D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374294CB-64C5-4AFB-A267-124F72A8FFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4992" yWindow="2760" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6804" yWindow="1248" windowWidth="22764" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
-  <si>
-    <t>测试项目编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
   <si>
     <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>读写超时，看interrupt和PSLVERR能否被拉起，而后拉起clear看能否清除interrupt，以及reg tree中regslv模块FSM的复位情况</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>测试层级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -259,6 +251,46 @@
   </si>
   <si>
     <t>reg_native_if transaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最上层APB下发请求时，reg_native_if各个信号的时序是否正确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外部memory读写超时，看interrupt和PSLVERR能否被拉起，而后拉起clear看能否清除interrupt，以及reg tree中regslv模块FSM的复位情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计进度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试用例标号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当读写请求的总线数据位宽和external memory位宽不一致时，实现snapshot机制保证读写的原子性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snapshot module</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -588,573 +620,821 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A40"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="112.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="120.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>17</v>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" t="s">
-        <v>17</v>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>17</v>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
         <v>16</v>
       </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
         <v>16</v>
       </c>
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
         <v>16</v>
       </c>
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
         <v>16</v>
       </c>
-      <c r="C34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" t="s">
-        <v>39</v>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" t="s">
-        <v>45</v>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>57</v>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test cases based on test plan
</commit_message>
<xml_diff>
--- a/docs/test_plan.xlsx
+++ b/docs/test_plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374294CB-64C5-4AFB-A267-124F72A8FFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6ECC26-AB5D-43A1-B53C-4ACA8EB9CCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6804" yWindow="1248" windowWidth="22764" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12216" yWindow="3144" windowWidth="18360" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
   <si>
     <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,26 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>field实例，在RDL中的sw属性为SW_RO，软件只读</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的sw属性为SW_RW，软件可读可写</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的sw属性为SW_RW1，软件可读可写，但只可写一次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的sw属性为SW_WO，软件只写</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的sw属性为SW_W1，软件只写，且只可写一次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>field实例，在RDL中的onread属性为NA，软件读取无side effect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -154,22 +134,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>field实例，在RDL中的hw属性为HW_RO，硬件只读，无法通过hw_value写入数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的hw属性为HW_RW，硬件可读可写</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的hw属性位HW_CLR，硬件访问时按位清零</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，在RDL中的hw属性位HW_SET，硬件访问时按位置位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>synchronous reset</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -210,14 +174,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>field实例，其属于的register在RDL中声明若干（一个或多个）alias register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field实例，其属于的register在RDL中声明若干（一个或多个）shared register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>field实例，其属于的register在RDL中同时声明了alias和shared</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -242,10 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>snapshot register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>内部bus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -286,11 +238,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>当读写请求的总线数据位宽和external memory位宽不一致时，实现snapshot机制保证读写的原子性</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>snapshot module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的sw属性为r (SW_RO)，软件只读</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的sw属性为rw (SW_RW)，软件可读可写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的sw属性为rw1 (SW_RW1)，软件可读可写，但只可写一次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的sw属性为w (SW_WO)，软件只写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的sw属性为w1 (SW_W1)，软件只写，且只可写一次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的hw属性为rw (HW_RW)，硬件可读可写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中的hw属性为r (HW_RO)，硬件只读，无法通过hw_value写入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中声明hwclr属性 (HW_CLR)，硬件访问时按位（写1）清零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，在RDL中声明hwset属性 (HW_SET)，硬件访问时按位（写1）置位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reset value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，定义不同的reset value，观察初始值、异步复位、同步复位时是否为reset value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snapshot memory access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snapshot register access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读写请求指向外部memory，且总线数据位宽和external memory位宽不一致时，实现snapshot机制保证读写的原子性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读写请求指向内部register，且总线数据位宽和internal register位宽不一致时，实现snapshot机制保证读写的原子性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，其属于的register在RDL中声明若干（一个或多个）alias register，具有不同的hj_syncresetsignal、sw、onread、onwrite属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>field实例，其属于的register在RDL中声明若干（一个或多个）shared register，具有不同的hj_syncresetsignal、sw、onread、onwrite属性</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -620,9 +636,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -636,10 +652,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
@@ -648,13 +664,13 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -662,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -671,7 +687,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -691,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -711,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -731,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -751,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -771,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -791,10 +807,10 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,16 +821,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -828,13 +844,13 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -842,7 +858,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -851,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -862,19 +878,19 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -891,10 +907,10 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -911,10 +927,10 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -931,10 +947,10 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -951,10 +967,10 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -971,10 +987,10 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,10 +1007,10 @@
         <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,10 +1027,10 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,10 +1047,10 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,10 +1067,10 @@
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,10 +1087,10 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1091,10 +1107,10 @@
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,10 +1127,10 @@
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,10 +1147,10 @@
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1151,10 +1167,10 @@
         <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,10 +1187,10 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1191,10 +1207,10 @@
         <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1211,10 +1227,10 @@
         <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1231,10 +1247,10 @@
         <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1251,10 +1267,10 @@
         <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1271,10 +1287,10 @@
         <v>16</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1291,10 +1307,10 @@
         <v>16</v>
       </c>
       <c r="E33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" t="s">
         <v>62</v>
-      </c>
-      <c r="F33" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,10 +1327,10 @@
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1328,13 +1344,13 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F35" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1348,13 +1364,13 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E36" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F36" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1368,53 +1384,53 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F37" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>60</v>
+      <c r="B38">
+        <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39">
-        <v>7</v>
+      <c r="B39" t="s">
+        <v>48</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1422,19 +1438,59 @@
         <v>39</v>
       </c>
       <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
         <v>8</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
         <v>67</v>
       </c>
-      <c r="D40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" t="s">
-        <v>66</v>
+      <c r="E42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test cases(need rebase)
</commit_message>
<xml_diff>
--- a/docs/test_plan.xlsx
+++ b/docs/test_plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6284F4-BD7B-4A7D-A797-DE49D89AFA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D32A11F-AE8E-4AF1-918F-C08F5FB10BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="1752" windowWidth="21204" windowHeight="13392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6564" yWindow="1188" windowWidth="21204" windowHeight="13392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
   <si>
     <t>描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -310,10 +310,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>读写请求指向内部register和外部memory时，发生不同时钟域的信号穿越</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1~8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -326,7 +322,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>在RDL中定义的skip_dff属性可以指定是否将读回来的数据打一拍，以改善时序约束</t>
+    <t>读写请求指向内部register和外部memory时，发生不同时钟域的信号穿越，需要对所有case验证有CDC和无CDC的结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在RDL中定义的skip_dff属性可以指定是否将读回来的数据打一拍，以改善时序约束，需要对所有case验证打拍和不打拍的结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -373,9 +373,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -663,7 +664,7 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
@@ -675,7 +676,7 @@
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -698,7 +699,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -718,7 +719,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -738,7 +739,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -758,7 +759,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -778,7 +779,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -798,7 +799,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -818,7 +819,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -838,7 +839,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -858,7 +859,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -878,7 +879,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -898,7 +899,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -918,7 +919,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -938,7 +939,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -958,7 +959,7 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -978,7 +979,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -998,7 +999,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1018,7 +1019,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1038,7 +1039,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1058,7 +1059,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1078,7 +1079,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1098,7 +1099,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1118,7 +1119,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1138,7 +1139,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1158,7 +1159,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1178,7 +1179,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1198,7 +1199,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>4</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1218,7 +1219,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1238,7 +1239,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1258,7 +1259,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1278,7 +1279,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>6</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1298,7 +1299,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1318,7 +1319,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1338,7 +1339,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1358,7 +1359,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1378,7 +1379,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1398,7 +1399,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1418,7 +1419,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1438,7 +1439,7 @@
       <c r="A39">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1458,7 +1459,7 @@
       <c r="A40">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>8</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1478,7 +1479,7 @@
       <c r="A41">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>8</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1498,8 +1499,8 @@
       <c r="A42">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
-        <v>73</v>
+      <c r="B42" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>69</v>
@@ -1511,18 +1512,21 @@
         <v>71</v>
       </c>
       <c r="F42" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="C43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" t="s">
         <v>74</v>
-      </c>
-      <c r="D43" t="s">
-        <v>75</v>
       </c>
       <c r="E43" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
fix rtl generation process
</commit_message>
<xml_diff>
--- a/docs/test_plan.xlsx
+++ b/docs/test_plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D32A11F-AE8E-4AF1-918F-C08F5FB10BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607E5844-F62E-4FB9-BF1C-B39FAA2B43E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6564" yWindow="1188" windowWidth="21204" windowHeight="13392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4296" yWindow="1116" windowWidth="22680" windowHeight="14376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>